<commit_message>
adding temp cond plots
</commit_message>
<xml_diff>
--- a/2 - Flow output Excel files - working drafts/Data Output 06_30_2019/Offsets and Clip times 06_30_2019.xlsx
+++ b/2 - Flow output Excel files - working drafts/Data Output 06_30_2019/Offsets and Clip times 06_30_2019.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="9336" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="9336"/>
   </bookViews>
   <sheets>
     <sheet name="Offsets" sheetId="1" r:id="rId1"/>
@@ -870,11 +870,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D26" sqref="D26"/>
+      <selection pane="bottomRight" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1353,6 +1353,15 @@
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>15</v>
+      </c>
+      <c r="B28" s="1">
+        <v>43634.40625</v>
+      </c>
+      <c r="C28" s="8">
+        <v>43738.999305555553</v>
+      </c>
+      <c r="D28">
+        <v>2.2000000000000002</v>
       </c>
       <c r="F28" s="26" t="b">
         <v>1</v>
@@ -18635,11 +18644,11 @@
   </sheetPr>
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B31" sqref="B31"/>
+      <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="24.9" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>